<commit_message>
add SRS_02 TC Ids
</commit_message>
<xml_diff>
--- a/Requirments/CAR_RTM .xlsx
+++ b/Requirments/CAR_RTM .xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="240">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -902,6 +902,13 @@
   <si>
     <t>Car_AdminRC_01</t>
   </si>
+  <si>
+    <t>Car_SearchTC_01
+Car_SearchTC_02
+Car_SearchTC_03
+Car_SearchTC_04
+Car_SearchTC_05</t>
+  </si>
 </sst>
 </file>
 
@@ -29740,8 +29747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C52" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29990,7 +29997,9 @@
       <c r="G7" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="41"/>
+      <c r="H7" s="41" t="s">
+        <v>239</v>
+      </c>
       <c r="I7" s="41"/>
       <c r="J7" s="41"/>
       <c r="K7" s="41"/>

</xml_diff>